<commit_message>
deleted cherry logo, add gantll chart and edited PCD
</commit_message>
<xml_diff>
--- a/Documentatie/Cheery Project Planning.xlsx
+++ b/Documentatie/Cheery Project Planning.xlsx
@@ -58,12 +58,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>Notes:</t>
-  </si>
-  <si>
-    <t>NOTES</t>
   </si>
   <si>
     <t>MONDAY</t>
@@ -79,6 +76,24 @@
   </si>
   <si>
     <t>END PROJECT!</t>
+  </si>
+  <si>
+    <t>PCD af</t>
+  </si>
+  <si>
+    <t>Begin of Defenitiestudie</t>
+  </si>
+  <si>
+    <t>Basis Ontwerp</t>
+  </si>
+  <si>
+    <t>BEGIN REALISATIE</t>
+  </si>
+  <si>
+    <t>IMPLEMENTATIE</t>
+  </si>
+  <si>
+    <t>DO</t>
   </si>
 </sst>
 </file>
@@ -187,7 +202,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +246,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -380,7 +401,7 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -426,11 +447,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
       <alignment horizontal="left" indent="7"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="left" indent="7"/>
+    <xf numFmtId="165" fontId="13" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -438,7 +456,22 @@
     <xf numFmtId="165" fontId="7" fillId="0" borderId="9" xfId="9" applyBorder="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="7" xfId="7" applyFill="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="6" xfId="7" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="9" borderId="8" xfId="7" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="13" fillId="9" borderId="7" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -662,8 +695,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="19050"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="19050"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -833,8 +866,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="7149192"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="7179608"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1004,8 +1037,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="14279336"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="14340168"/>
+          <a:ext cx="466725" cy="1186478"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1175,8 +1208,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="21409479"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="21500726"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1346,8 +1379,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="28539621"/>
-          <a:ext cx="466725" cy="1183278"/>
+          <a:off x="168088" y="28661285"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1517,8 +1550,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="35669764"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="35821844"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1688,8 +1721,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="42799907"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="42982403"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -1859,8 +1892,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="49930050"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="50142962"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -2030,8 +2063,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="57060193"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="57303521"/>
+          <a:ext cx="466725" cy="1186478"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -2201,8 +2234,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="176893" y="64190336"/>
-          <a:ext cx="466725" cy="1183277"/>
+          <a:off x="168088" y="64464079"/>
+          <a:ext cx="466725" cy="1186479"/>
           <a:chOff x="371475" y="0"/>
           <a:chExt cx="457200" cy="990600"/>
         </a:xfrm>
@@ -2588,8 +2621,8 @@
   </sheetPr>
   <dimension ref="A1:I150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2604,11 +2637,11 @@
       <c r="A1" s="12">
         <v>2015</v>
       </c>
-      <c r="B1" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
+      <c r="B1" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2624,7 +2657,7 @@
     <row r="3" spans="1:9" s="3" customFormat="1" ht="14.25" customHeight="1">
       <c r="A3" s="2"/>
       <c r="B3" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="13" t="str">
         <f>UPPER(TEXT(C4,"dddd"))</f>
@@ -2651,7 +2684,7 @@
         <v>SUNDAY</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
@@ -2686,7 +2719,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="16.5" customHeight="1">
@@ -2716,9 +2749,13 @@
     <row r="7" spans="1:9" ht="56.25" customHeight="1">
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
+      <c r="D7" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="G7" s="7"/>
       <c r="H7" s="9"/>
     </row>
@@ -2751,7 +2788,9 @@
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="G9" s="7"/>
       <c r="H9" s="9"/>
     </row>
@@ -2784,7 +2823,9 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="7" t="s">
+        <v>11</v>
+      </c>
       <c r="G11" s="7"/>
       <c r="H11" s="9"/>
     </row>
@@ -2829,22 +2870,22 @@
       <c r="C14" s="6">
         <v>42311</v>
       </c>
-      <c r="D14" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14" s="18"/>
-      <c r="F14" s="18"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="18"/>
+      <c r="D14" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
     </row>
     <row r="15" spans="1:9" ht="63.75" customHeight="1">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="15"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A16" s="12">
@@ -2991,13 +3032,15 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" customHeight="1">
       <c r="B25" s="6">
@@ -3024,13 +3067,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
-      <c r="H26" s="9"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1">
       <c r="B27" s="6">
@@ -3057,13 +3100,13 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="57" customHeight="1">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="10"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="22"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
       <c r="B29" s="6">
@@ -3073,22 +3116,22 @@
       <c r="C29" s="6">
         <v>42339</v>
       </c>
-      <c r="D29" s="17" t="s">
+      <c r="D29" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="18"/>
-      <c r="F29" s="18"/>
-      <c r="G29" s="18"/>
-      <c r="H29" s="18"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="17"/>
     </row>
     <row r="30" spans="1:8" ht="63.75" customHeight="1">
-      <c r="B30" s="7"/>
+      <c r="B30" s="20"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="15"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A31" s="12">
@@ -3170,12 +3213,12 @@
     </row>
     <row r="35" spans="1:8" ht="56.25" customHeight="1">
       <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="9"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1">
       <c r="B36" s="6">
@@ -3202,13 +3245,15 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="9"/>
+      <c r="B37" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" customHeight="1">
       <c r="B38" s="6">
@@ -3235,9 +3280,9 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B39" s="7"/>
-      <c r="C39" s="19" t="s">
-        <v>6</v>
+      <c r="B39" s="20"/>
+      <c r="C39" s="15" t="s">
+        <v>5</v>
       </c>
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
@@ -3319,22 +3364,22 @@
       <c r="C44" s="6">
         <v>42374</v>
       </c>
-      <c r="D44" s="17" t="s">
+      <c r="D44" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="18"/>
-      <c r="F44" s="18"/>
-      <c r="G44" s="18"/>
-      <c r="H44" s="18"/>
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
     </row>
     <row r="45" spans="1:8" ht="63.75" customHeight="1">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
-      <c r="G45" s="15"/>
-      <c r="H45" s="15"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="18"/>
+      <c r="F45" s="18"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="18"/>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A46" s="12">
@@ -3563,22 +3608,22 @@
       <c r="C59" s="6">
         <v>42402</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="D59" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="18"/>
-      <c r="F59" s="18"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
+      <c r="E59" s="17"/>
+      <c r="F59" s="17"/>
+      <c r="G59" s="17"/>
+      <c r="H59" s="17"/>
     </row>
     <row r="60" spans="1:8" ht="63.75" customHeight="1">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="15"/>
-      <c r="F60" s="15"/>
-      <c r="G60" s="15"/>
-      <c r="H60" s="15"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="18"/>
+      <c r="F60" s="18"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="18"/>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A61" s="12">
@@ -3807,22 +3852,22 @@
       <c r="C74" s="6">
         <v>42437</v>
       </c>
-      <c r="D74" s="17" t="s">
+      <c r="D74" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="18"/>
-      <c r="F74" s="18"/>
-      <c r="G74" s="18"/>
-      <c r="H74" s="18"/>
+      <c r="E74" s="17"/>
+      <c r="F74" s="17"/>
+      <c r="G74" s="17"/>
+      <c r="H74" s="17"/>
     </row>
     <row r="75" spans="1:8" ht="63.75" customHeight="1">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
-      <c r="D75" s="15"/>
-      <c r="E75" s="15"/>
-      <c r="F75" s="15"/>
-      <c r="G75" s="15"/>
-      <c r="H75" s="15"/>
+      <c r="D75" s="18"/>
+      <c r="E75" s="18"/>
+      <c r="F75" s="18"/>
+      <c r="G75" s="18"/>
+      <c r="H75" s="18"/>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A76" s="12">
@@ -4051,22 +4096,22 @@
       <c r="C89" s="6">
         <v>42465</v>
       </c>
-      <c r="D89" s="17" t="s">
+      <c r="D89" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E89" s="18"/>
-      <c r="F89" s="18"/>
-      <c r="G89" s="18"/>
-      <c r="H89" s="18"/>
+      <c r="E89" s="17"/>
+      <c r="F89" s="17"/>
+      <c r="G89" s="17"/>
+      <c r="H89" s="17"/>
     </row>
     <row r="90" spans="1:8" ht="63.75" customHeight="1">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="15"/>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-      <c r="G90" s="15"/>
-      <c r="H90" s="15"/>
+      <c r="D90" s="18"/>
+      <c r="E90" s="18"/>
+      <c r="F90" s="18"/>
+      <c r="G90" s="18"/>
+      <c r="H90" s="18"/>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A91" s="12">
@@ -4295,22 +4340,22 @@
       <c r="C104" s="6">
         <v>42493</v>
       </c>
-      <c r="D104" s="17" t="s">
+      <c r="D104" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E104" s="18"/>
-      <c r="F104" s="18"/>
-      <c r="G104" s="18"/>
-      <c r="H104" s="18"/>
+      <c r="E104" s="17"/>
+      <c r="F104" s="17"/>
+      <c r="G104" s="17"/>
+      <c r="H104" s="17"/>
     </row>
     <row r="105" spans="1:8" ht="63.75" customHeight="1">
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
-      <c r="D105" s="15"/>
-      <c r="E105" s="15"/>
-      <c r="F105" s="15"/>
-      <c r="G105" s="15"/>
-      <c r="H105" s="15"/>
+      <c r="D105" s="18"/>
+      <c r="E105" s="18"/>
+      <c r="F105" s="18"/>
+      <c r="G105" s="18"/>
+      <c r="H105" s="18"/>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A106" s="12">
@@ -4539,22 +4584,22 @@
       <c r="C119" s="6">
         <v>42521</v>
       </c>
-      <c r="D119" s="17" t="s">
+      <c r="D119" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E119" s="18"/>
-      <c r="F119" s="18"/>
-      <c r="G119" s="18"/>
-      <c r="H119" s="18"/>
+      <c r="E119" s="17"/>
+      <c r="F119" s="17"/>
+      <c r="G119" s="17"/>
+      <c r="H119" s="17"/>
     </row>
     <row r="120" spans="1:8" ht="63.75" customHeight="1">
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
-      <c r="D120" s="15"/>
-      <c r="E120" s="15"/>
-      <c r="F120" s="15"/>
-      <c r="G120" s="15"/>
-      <c r="H120" s="15"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="18"/>
+      <c r="F120" s="18"/>
+      <c r="G120" s="18"/>
+      <c r="H120" s="18"/>
     </row>
     <row r="121" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A121" s="12">
@@ -4783,22 +4828,22 @@
       <c r="C134" s="6">
         <v>42556</v>
       </c>
-      <c r="D134" s="17" t="s">
+      <c r="D134" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="18"/>
-      <c r="F134" s="18"/>
-      <c r="G134" s="18"/>
-      <c r="H134" s="18"/>
+      <c r="E134" s="17"/>
+      <c r="F134" s="17"/>
+      <c r="G134" s="17"/>
+      <c r="H134" s="17"/>
     </row>
     <row r="135" spans="1:8" ht="63.75" customHeight="1">
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
-      <c r="D135" s="15"/>
-      <c r="E135" s="15"/>
-      <c r="F135" s="15"/>
-      <c r="G135" s="15"/>
-      <c r="H135" s="15"/>
+      <c r="D135" s="18"/>
+      <c r="E135" s="18"/>
+      <c r="F135" s="18"/>
+      <c r="G135" s="18"/>
+      <c r="H135" s="18"/>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A136" s="12">
@@ -5027,30 +5072,25 @@
       <c r="C149" s="6">
         <v>42584</v>
       </c>
-      <c r="D149" s="17" t="s">
+      <c r="D149" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E149" s="18"/>
-      <c r="F149" s="18"/>
-      <c r="G149" s="18"/>
-      <c r="H149" s="18"/>
+      <c r="E149" s="17"/>
+      <c r="F149" s="17"/>
+      <c r="G149" s="17"/>
+      <c r="H149" s="17"/>
     </row>
     <row r="150" spans="2:8" ht="63.75" customHeight="1">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
-      <c r="D150" s="15"/>
-      <c r="E150" s="15"/>
-      <c r="F150" s="15"/>
-      <c r="G150" s="15"/>
-      <c r="H150" s="15"/>
+      <c r="D150" s="18"/>
+      <c r="E150" s="18"/>
+      <c r="F150" s="18"/>
+      <c r="G150" s="18"/>
+      <c r="H150" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="D149:H149"/>
-    <mergeCell ref="D150:H150"/>
-    <mergeCell ref="D135:H135"/>
-    <mergeCell ref="D119:H119"/>
-    <mergeCell ref="D134:H134"/>
     <mergeCell ref="D105:H105"/>
     <mergeCell ref="D120:H120"/>
     <mergeCell ref="B1:D1"/>
@@ -5067,6 +5107,11 @@
     <mergeCell ref="D89:H89"/>
     <mergeCell ref="D104:H104"/>
     <mergeCell ref="D90:H90"/>
+    <mergeCell ref="D149:H149"/>
+    <mergeCell ref="D150:H150"/>
+    <mergeCell ref="D135:H135"/>
+    <mergeCell ref="D119:H119"/>
+    <mergeCell ref="D134:H134"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:H4 B6:H6 B8:H8 B10:H10 B12:H12 B14:C14">

</xml_diff>

<commit_message>
changed Network Diagram, Changed PCD
</commit_message>
<xml_diff>
--- a/Documentatie/Cheery Project Planning.xlsx
+++ b/Documentatie/Cheery Project Planning.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Notes:</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>DO</t>
+  </si>
+  <si>
+    <t>Defenitie Studie Done</t>
   </si>
 </sst>
 </file>
@@ -450,18 +453,6 @@
     <xf numFmtId="165" fontId="13" fillId="8" borderId="7" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="9" xfId="9" applyBorder="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="8">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
-      <alignment horizontal="left" indent="7"/>
-    </xf>
     <xf numFmtId="165" fontId="9" fillId="9" borderId="7" xfId="7" applyFill="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -473,6 +464,18 @@
     </xf>
     <xf numFmtId="165" fontId="13" fillId="9" borderId="7" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="8">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="10">
+      <alignment horizontal="left" indent="7"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="9" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="9" xfId="9" applyBorder="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -2622,7 +2625,7 @@
   <dimension ref="A1:I150"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -2637,11 +2640,11 @@
       <c r="A1" s="12">
         <v>2015</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
@@ -2787,7 +2790,9 @@
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F9" s="7" t="s">
         <v>8</v>
       </c>
@@ -2870,22 +2875,22 @@
       <c r="C14" s="6">
         <v>42311</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="17"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
     </row>
     <row r="15" spans="1:9" ht="63.75" customHeight="1">
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="18"/>
-      <c r="E15" s="18"/>
-      <c r="F15" s="18"/>
-      <c r="G15" s="18"/>
-      <c r="H15" s="18"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:9" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A16" s="12">
@@ -3032,15 +3037,15 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="21"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="17"/>
     </row>
     <row r="25" spans="1:8" ht="16.5" customHeight="1">
       <c r="B25" s="6">
@@ -3067,13 +3072,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="21"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="16"/>
+      <c r="H26" s="17"/>
     </row>
     <row r="27" spans="1:8" ht="16.5" customHeight="1">
       <c r="B27" s="6">
@@ -3100,13 +3105,13 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="57" customHeight="1">
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="22"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="18"/>
     </row>
     <row r="29" spans="1:8" ht="16.5" customHeight="1">
       <c r="B29" s="6">
@@ -3116,22 +3121,22 @@
       <c r="C29" s="6">
         <v>42339</v>
       </c>
-      <c r="D29" s="16" t="s">
+      <c r="D29" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="17"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
     </row>
     <row r="30" spans="1:8" ht="63.75" customHeight="1">
-      <c r="B30" s="20"/>
+      <c r="B30" s="16"/>
       <c r="C30" s="7"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="18"/>
-      <c r="H30" s="18"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20"/>
     </row>
     <row r="31" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A31" s="12">
@@ -3213,12 +3218,12 @@
     </row>
     <row r="35" spans="1:8" ht="56.25" customHeight="1">
       <c r="B35" s="7"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
-      <c r="G35" s="20"/>
-      <c r="H35" s="21"/>
+      <c r="C35" s="16"/>
+      <c r="D35" s="16"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="16"/>
+      <c r="H35" s="17"/>
     </row>
     <row r="36" spans="1:8" ht="16.5" customHeight="1">
       <c r="B36" s="6">
@@ -3245,15 +3250,15 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B37" s="23" t="s">
+      <c r="B37" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
-      <c r="G37" s="20"/>
-      <c r="H37" s="21"/>
+      <c r="C37" s="16"/>
+      <c r="D37" s="16"/>
+      <c r="E37" s="16"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="16"/>
+      <c r="H37" s="17"/>
     </row>
     <row r="38" spans="1:8" ht="16.5" customHeight="1">
       <c r="B38" s="6">
@@ -3280,7 +3285,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="56.25" customHeight="1">
-      <c r="B39" s="20"/>
+      <c r="B39" s="16"/>
       <c r="C39" s="15" t="s">
         <v>5</v>
       </c>
@@ -3364,22 +3369,22 @@
       <c r="C44" s="6">
         <v>42374</v>
       </c>
-      <c r="D44" s="16" t="s">
+      <c r="D44" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E44" s="17"/>
-      <c r="F44" s="17"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
     </row>
     <row r="45" spans="1:8" ht="63.75" customHeight="1">
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
-      <c r="D45" s="18"/>
-      <c r="E45" s="18"/>
-      <c r="F45" s="18"/>
-      <c r="G45" s="18"/>
-      <c r="H45" s="18"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
     </row>
     <row r="46" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A46" s="12">
@@ -3608,22 +3613,22 @@
       <c r="C59" s="6">
         <v>42402</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E59" s="17"/>
-      <c r="F59" s="17"/>
-      <c r="G59" s="17"/>
-      <c r="H59" s="17"/>
+      <c r="E59" s="23"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="23"/>
     </row>
     <row r="60" spans="1:8" ht="63.75" customHeight="1">
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
-      <c r="D60" s="18"/>
-      <c r="E60" s="18"/>
-      <c r="F60" s="18"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
+      <c r="D60" s="20"/>
+      <c r="E60" s="20"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="20"/>
+      <c r="H60" s="20"/>
     </row>
     <row r="61" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A61" s="12">
@@ -3852,22 +3857,22 @@
       <c r="C74" s="6">
         <v>42437</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E74" s="17"/>
-      <c r="F74" s="17"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
+      <c r="E74" s="23"/>
+      <c r="F74" s="23"/>
+      <c r="G74" s="23"/>
+      <c r="H74" s="23"/>
     </row>
     <row r="75" spans="1:8" ht="63.75" customHeight="1">
       <c r="B75" s="7"/>
       <c r="C75" s="7"/>
-      <c r="D75" s="18"/>
-      <c r="E75" s="18"/>
-      <c r="F75" s="18"/>
-      <c r="G75" s="18"/>
-      <c r="H75" s="18"/>
+      <c r="D75" s="20"/>
+      <c r="E75" s="20"/>
+      <c r="F75" s="20"/>
+      <c r="G75" s="20"/>
+      <c r="H75" s="20"/>
     </row>
     <row r="76" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A76" s="12">
@@ -4096,22 +4101,22 @@
       <c r="C89" s="6">
         <v>42465</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E89" s="17"/>
-      <c r="F89" s="17"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
+      <c r="E89" s="23"/>
+      <c r="F89" s="23"/>
+      <c r="G89" s="23"/>
+      <c r="H89" s="23"/>
     </row>
     <row r="90" spans="1:8" ht="63.75" customHeight="1">
       <c r="B90" s="7"/>
       <c r="C90" s="7"/>
-      <c r="D90" s="18"/>
-      <c r="E90" s="18"/>
-      <c r="F90" s="18"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
+      <c r="D90" s="20"/>
+      <c r="E90" s="20"/>
+      <c r="F90" s="20"/>
+      <c r="G90" s="20"/>
+      <c r="H90" s="20"/>
     </row>
     <row r="91" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A91" s="12">
@@ -4340,22 +4345,22 @@
       <c r="C104" s="6">
         <v>42493</v>
       </c>
-      <c r="D104" s="16" t="s">
+      <c r="D104" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E104" s="17"/>
-      <c r="F104" s="17"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
+      <c r="E104" s="23"/>
+      <c r="F104" s="23"/>
+      <c r="G104" s="23"/>
+      <c r="H104" s="23"/>
     </row>
     <row r="105" spans="1:8" ht="63.75" customHeight="1">
       <c r="B105" s="7"/>
       <c r="C105" s="7"/>
-      <c r="D105" s="18"/>
-      <c r="E105" s="18"/>
-      <c r="F105" s="18"/>
-      <c r="G105" s="18"/>
-      <c r="H105" s="18"/>
+      <c r="D105" s="20"/>
+      <c r="E105" s="20"/>
+      <c r="F105" s="20"/>
+      <c r="G105" s="20"/>
+      <c r="H105" s="20"/>
     </row>
     <row r="106" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A106" s="12">
@@ -4584,22 +4589,22 @@
       <c r="C119" s="6">
         <v>42521</v>
       </c>
-      <c r="D119" s="16" t="s">
+      <c r="D119" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E119" s="17"/>
-      <c r="F119" s="17"/>
-      <c r="G119" s="17"/>
-      <c r="H119" s="17"/>
+      <c r="E119" s="23"/>
+      <c r="F119" s="23"/>
+      <c r="G119" s="23"/>
+      <c r="H119" s="23"/>
     </row>
     <row r="120" spans="1:8" ht="63.75" customHeight="1">
       <c r="B120" s="7"/>
       <c r="C120" s="7"/>
-      <c r="D120" s="18"/>
-      <c r="E120" s="18"/>
-      <c r="F120" s="18"/>
-      <c r="G120" s="18"/>
-      <c r="H120" s="18"/>
+      <c r="D120" s="20"/>
+      <c r="E120" s="20"/>
+      <c r="F120" s="20"/>
+      <c r="G120" s="20"/>
+      <c r="H120" s="20"/>
     </row>
     <row r="121" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A121" s="12">
@@ -4828,22 +4833,22 @@
       <c r="C134" s="6">
         <v>42556</v>
       </c>
-      <c r="D134" s="16" t="s">
+      <c r="D134" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E134" s="17"/>
-      <c r="F134" s="17"/>
-      <c r="G134" s="17"/>
-      <c r="H134" s="17"/>
+      <c r="E134" s="23"/>
+      <c r="F134" s="23"/>
+      <c r="G134" s="23"/>
+      <c r="H134" s="23"/>
     </row>
     <row r="135" spans="1:8" ht="63.75" customHeight="1">
       <c r="B135" s="7"/>
       <c r="C135" s="7"/>
-      <c r="D135" s="18"/>
-      <c r="E135" s="18"/>
-      <c r="F135" s="18"/>
-      <c r="G135" s="18"/>
-      <c r="H135" s="18"/>
+      <c r="D135" s="20"/>
+      <c r="E135" s="20"/>
+      <c r="F135" s="20"/>
+      <c r="G135" s="20"/>
+      <c r="H135" s="20"/>
     </row>
     <row r="136" spans="1:8" s="1" customFormat="1" ht="54" customHeight="1">
       <c r="A136" s="12">
@@ -5072,25 +5077,30 @@
       <c r="C149" s="6">
         <v>42584</v>
       </c>
-      <c r="D149" s="16" t="s">
+      <c r="D149" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="E149" s="17"/>
-      <c r="F149" s="17"/>
-      <c r="G149" s="17"/>
-      <c r="H149" s="17"/>
+      <c r="E149" s="23"/>
+      <c r="F149" s="23"/>
+      <c r="G149" s="23"/>
+      <c r="H149" s="23"/>
     </row>
     <row r="150" spans="2:8" ht="63.75" customHeight="1">
       <c r="B150" s="7"/>
       <c r="C150" s="7"/>
-      <c r="D150" s="18"/>
-      <c r="E150" s="18"/>
-      <c r="F150" s="18"/>
-      <c r="G150" s="18"/>
-      <c r="H150" s="18"/>
+      <c r="D150" s="20"/>
+      <c r="E150" s="20"/>
+      <c r="F150" s="20"/>
+      <c r="G150" s="20"/>
+      <c r="H150" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="D149:H149"/>
+    <mergeCell ref="D150:H150"/>
+    <mergeCell ref="D135:H135"/>
+    <mergeCell ref="D119:H119"/>
+    <mergeCell ref="D134:H134"/>
     <mergeCell ref="D105:H105"/>
     <mergeCell ref="D120:H120"/>
     <mergeCell ref="B1:D1"/>
@@ -5107,11 +5117,6 @@
     <mergeCell ref="D89:H89"/>
     <mergeCell ref="D104:H104"/>
     <mergeCell ref="D90:H90"/>
-    <mergeCell ref="D149:H149"/>
-    <mergeCell ref="D150:H150"/>
-    <mergeCell ref="D135:H135"/>
-    <mergeCell ref="D119:H119"/>
-    <mergeCell ref="D134:H134"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B4:H4 B6:H6 B8:H8 B10:H10 B12:H12 B14:C14">

</xml_diff>